<commit_message>
bug fixes and Randstad_car_times.xlsx adjustment
</commit_message>
<xml_diff>
--- a/Data_files/Randstad_car_times.xlsx
+++ b/Data_files/Randstad_car_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1449AD91-5FEC-44ED-AA3D-80FCED0BD018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909987ED-CB43-424D-9919-DD5214BE0F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="23">
   <si>
     <t>Cities</t>
   </si>
@@ -490,7 +512,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,65 +592,66 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>22</v>
+      <c r="C2" s="3" t="str" cm="1">
+        <f t="array" ref="C2:V2">TRANSPOSE(B3:B22)</f>
+        <v>x</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="E2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="K2" s="3">
         <v>26</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>22</v>
+      <c r="L2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="M2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="N2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="O2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="R2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S2" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T2" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="U2" s="3">
         <v>24</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>22</v>
+      <c r="V2" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -641,8 +664,9 @@
       <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
+      <c r="D3" s="3" t="str" cm="1">
+        <f t="array" ref="D3:V3">TRANSPOSE(C4:C22)</f>
+        <v>x</v>
       </c>
       <c r="E3" s="3">
         <v>37</v>
@@ -650,53 +674,53 @@
       <c r="F3" s="3">
         <v>28</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>22</v>
+      <c r="G3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="J3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="K3" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="L3" s="3">
         <v>26</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>22</v>
+      <c r="M3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="N3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="O3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="R3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U3" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V3" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -712,56 +736,57 @@
       <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
+      <c r="E4" s="3" t="str" cm="1">
+        <f t="array" ref="E4:V4">TRANSPOSE(D5:D22)</f>
+        <v>x</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="G4" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="H4" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="I4" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="J4" s="3">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="L4" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="M4" s="3">
         <v>19</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>22</v>
+      <c r="N4" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="O4" s="3">
         <v>19</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>22</v>
+      <c r="P4" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q4" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="R4" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S4" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="T4" s="3">
         <v>22</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>22</v>
+      <c r="U4" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="V4" s="3">
         <v>22</v>
@@ -783,56 +808,57 @@
       <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="3" cm="1">
+        <f t="array" ref="F5:V5">TRANSPOSE(E6:E22)</f>
         <v>38</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>22</v>
+      <c r="G5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="I5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="J5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="K5" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="L5" s="3">
         <v>23</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>22</v>
+      <c r="M5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="N5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="O5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P5" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="Q5" s="3">
         <v>23</v>
       </c>
-      <c r="R5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>22</v>
+      <c r="R5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U5" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V5" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -854,17 +880,18 @@
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>22</v>
+      <c r="G6" s="3" t="str" cm="1">
+        <f t="array" ref="G6:V6">TRANSPOSE(F7:F22)</f>
+        <v>x</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="J6" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="K6" s="3">
         <v>25</v>
@@ -872,26 +899,26 @@
       <c r="L6" s="3">
         <v>29</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>22</v>
+      <c r="M6" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="N6" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="O6" s="3">
         <v>21</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>22</v>
+      <c r="P6" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="Q6" s="3">
         <v>40</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>22</v>
+      <c r="R6" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S6" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="T6" s="3">
         <v>41</v>
@@ -899,8 +926,8 @@
       <c r="U6" s="3">
         <v>16</v>
       </c>
-      <c r="V6" s="3" t="s">
-        <v>22</v>
+      <c r="V6" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -925,35 +952,36 @@
       <c r="G7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="3" cm="1">
+        <f t="array" ref="H7:V7">TRANSPOSE(G8:G22)</f>
         <v>20</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>22</v>
+      <c r="I7" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="J7" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="K7" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="M7" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="N7" s="3">
         <v>19</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>22</v>
+      <c r="O7" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P7" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q7" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="R7" s="3">
         <v>18</v>
@@ -961,11 +989,11 @@
       <c r="S7" s="3">
         <v>19</v>
       </c>
-      <c r="T7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>22</v>
+      <c r="T7" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U7" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="V7" s="3">
         <v>21</v>
@@ -996,44 +1024,45 @@
       <c r="H8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>22</v>
+      <c r="I8" s="3" t="str" cm="1">
+        <f t="array" ref="I8:V8">TRANSPOSE(H9:H22)</f>
+        <v>x</v>
+      </c>
+      <c r="J8" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="K8" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="L8" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="M8" s="3">
         <v>23</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>22</v>
+      <c r="N8" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="O8" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P8" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q8" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="R8" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="S8" s="3">
         <v>18</v>
       </c>
-      <c r="T8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>22</v>
+      <c r="T8" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U8" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="V8" s="3">
         <v>18</v>
@@ -1067,44 +1096,45 @@
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>22</v>
+      <c r="J9" s="3" t="str" cm="1">
+        <f t="array" ref="J9:V9">TRANSPOSE(I10:I22)</f>
+        <v>x</v>
+      </c>
+      <c r="K9" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="L9" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="M9" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="N9" s="3">
         <v>27</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>22</v>
+      <c r="O9" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P9" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="Q9" s="3">
         <v>44</v>
       </c>
-      <c r="R9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>22</v>
+      <c r="R9" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S9" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T9" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U9" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V9" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1117,8 +1147,8 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
+      <c r="D10" s="1">
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>22</v>
@@ -1138,38 +1168,39 @@
       <c r="J10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>22</v>
+      <c r="K10" s="3" t="str" cm="1">
+        <f t="array" ref="K10:V10">TRANSPOSE(J11:J22)</f>
+        <v>x</v>
+      </c>
+      <c r="L10" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="M10" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="N10" s="3">
         <v>25</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>22</v>
+      <c r="O10" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P10" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q10" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="R10" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S10" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="T10" s="3">
         <v>21</v>
       </c>
-      <c r="U10" s="3" t="s">
-        <v>22</v>
+      <c r="U10" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="V10" s="3">
         <v>20</v>
@@ -1209,38 +1240,39 @@
       <c r="K11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>22</v>
+      <c r="L11" s="3" t="str" cm="1">
+        <f t="array" ref="L11:V11">TRANSPOSE(K12:K22)</f>
+        <v>x</v>
       </c>
       <c r="M11" s="3">
         <v>37</v>
       </c>
-      <c r="N11" s="3" t="s">
-        <v>22</v>
+      <c r="N11" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="O11" s="3">
         <v>19</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>22</v>
+      <c r="P11" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q11" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="R11" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S11" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T11" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="U11" s="3">
         <v>30</v>
       </c>
-      <c r="V11" s="3" t="s">
-        <v>22</v>
+      <c r="V11" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1280,35 +1312,36 @@
       <c r="L12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>22</v>
+      <c r="M12" s="3" t="str" cm="1">
+        <f t="array" ref="M12:V12">TRANSPOSE(L13:L22)</f>
+        <v>x</v>
+      </c>
+      <c r="N12" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="O12" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="P12" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="Q12" s="3">
         <v>22</v>
       </c>
-      <c r="R12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>22</v>
+      <c r="R12" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S12" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T12" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U12" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V12" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1351,29 +1384,30 @@
       <c r="M13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>22</v>
+      <c r="N13" s="3" t="str" cm="1">
+        <f t="array" ref="N13:V13">TRANSPOSE(M14:M22)</f>
+        <v>x</v>
       </c>
       <c r="O13" s="3">
         <v>20</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>22</v>
+      <c r="P13" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q13" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="R13" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S13" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T13" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U13" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="V13" s="3">
         <v>19</v>
@@ -1422,26 +1456,27 @@
       <c r="N14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>22</v>
+      <c r="O14" s="3" t="str" cm="1">
+        <f t="array" ref="O14:V14">TRANSPOSE(N15:N22)</f>
+        <v>x</v>
       </c>
       <c r="P14" s="3">
         <v>21</v>
       </c>
-      <c r="Q14" s="3" t="s">
-        <v>22</v>
+      <c r="Q14" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="R14" s="3">
         <v>15</v>
       </c>
-      <c r="S14" s="3">
-        <v>23</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>22</v>
+      <c r="S14" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T14" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U14" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="V14" s="3">
         <v>24</v>
@@ -1493,26 +1528,27 @@
       <c r="O15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>22</v>
+      <c r="P15" s="3" t="str" cm="1">
+        <f t="array" ref="P15:V15">TRANSPOSE(O16:O22)</f>
+        <v>x</v>
       </c>
       <c r="Q15" s="3">
         <v>41</v>
       </c>
-      <c r="R15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>22</v>
+      <c r="R15" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="S15" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="T15" s="3">
         <v>41</v>
       </c>
-      <c r="U15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V15" s="3" t="s">
-        <v>22</v>
+      <c r="U15" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V15" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1564,23 +1600,24 @@
       <c r="P16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q16" s="3" t="s">
-        <v>22</v>
+      <c r="Q16" s="3" t="str" cm="1">
+        <f t="array" ref="Q16:V16">TRANSPOSE(P17:P22)</f>
+        <v>x</v>
       </c>
       <c r="R16" s="3">
         <v>14</v>
       </c>
-      <c r="S16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V16" s="3" t="s">
-        <v>22</v>
+      <c r="S16" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="T16" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U16" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V16" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1635,20 +1672,21 @@
       <c r="Q17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>22</v>
+      <c r="R17" s="3" t="str" cm="1">
+        <f t="array" ref="R17:V17">TRANSPOSE(Q18:Q22)</f>
+        <v>x</v>
+      </c>
+      <c r="S17" s="3" t="str">
+        <v>x</v>
       </c>
       <c r="T17" s="3">
         <v>25</v>
       </c>
-      <c r="U17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V17" s="3" t="s">
-        <v>22</v>
+      <c r="U17" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V17" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1706,17 +1744,18 @@
       <c r="R18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S18" s="3">
+      <c r="S18" s="3" cm="1">
+        <f t="array" ref="S18:V18">TRANSPOSE(R19:R22)</f>
         <v>19</v>
       </c>
-      <c r="T18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V18" s="3" t="s">
-        <v>22</v>
+      <c r="T18" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="U18" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V18" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1777,14 +1816,15 @@
       <c r="S19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V19" s="3" t="s">
-        <v>22</v>
+      <c r="T19" s="3" t="str" cm="1">
+        <f t="array" ref="T19:V19">TRANSPOSE(S20:S22)</f>
+        <v>x</v>
+      </c>
+      <c r="U19" s="3" t="str">
+        <v>x</v>
+      </c>
+      <c r="V19" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1848,11 +1888,12 @@
       <c r="T20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V20" s="3" t="s">
-        <v>22</v>
+      <c r="U20" s="3" t="str" cm="1">
+        <f t="array" ref="U20:V20">TRANSPOSE(T21:T22)</f>
+        <v>x</v>
+      </c>
+      <c r="V20" s="3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1919,8 +1960,9 @@
       <c r="U21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V21" s="3" t="s">
-        <v>22</v>
+      <c r="V21" s="3" t="str" cm="1">
+        <f t="array" ref="V21">TRANSPOSE(U22)</f>
+        <v>x</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -1997,15 +2039,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2149,6 +2182,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2156,14 +2198,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FF02CE3-2C5B-42A9-AA67-1B9085842FBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E3DCCEF-2FC0-4346-9588-18F66903106E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2177,6 +2211,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FF02CE3-2C5B-42A9-AA67-1B9085842FBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
more minor adjustments to the graph
</commit_message>
<xml_diff>
--- a/Data_files/Randstad_car_times.xlsx
+++ b/Data_files/Randstad_car_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909987ED-CB43-424D-9919-DD5214BE0F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD36A57-9AEA-4A6B-BD32-EEF3746FC716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -768,7 +768,7 @@
         <v>x</v>
       </c>
       <c r="O4" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="P4" s="3" t="str">
         <v>x</v>
@@ -1493,7 +1493,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>22</v>
@@ -2039,6 +2039,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2182,22 +2197,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B52927-EB1B-4D32-8C26-F724208F026A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FF02CE3-2C5B-42A9-AA67-1B9085842FBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E3DCCEF-2FC0-4346-9588-18F66903106E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2213,28 +2237,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FF02CE3-2C5B-42A9-AA67-1B9085842FBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B52927-EB1B-4D32-8C26-F724208F026A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
completed the car network adjacency
</commit_message>
<xml_diff>
--- a/Data_files/Randstad_car_times.xlsx
+++ b/Data_files/Randstad_car_times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3503A05-FC30-40E0-BE3B-156BE300E184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44B8CC4-9E0B-45DF-803E-36F3781DB022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="H7" s="7" cm="1">
         <f t="array" ref="H7:W7">TRANSPOSE(G8:G23)</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I7" s="7" t="str">
         <v>x</v>
@@ -1130,7 +1130,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="6">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>22</v>
@@ -2267,21 +2267,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2425,31 +2410,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B52927-EB1B-4D32-8C26-F724208F026A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FF02CE3-2C5B-42A9-AA67-1B9085842FBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E3DCCEF-2FC0-4346-9588-18F66903106E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2465,4 +2441,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FF02CE3-2C5B-42A9-AA67-1B9085842FBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41B52927-EB1B-4D32-8C26-F724208F026A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>